<commit_message>
adda new custom action to terminate the sever
</commit_message>
<xml_diff>
--- a/rasaproject8/user_data.xlsx
+++ b/rasaproject8/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,14 +531,44 @@
           <t>kalhara</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0753999382</t>
-        </is>
+      <c r="B7" t="n">
+        <v>753999382</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>my phone hase no signal at all,and router also not working there is a blinking red lite on los</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>chulanjana</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>200031233443434</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>my phone is not working there is no signal at all</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>3323e32e342</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>0382250162</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>my phone is not working</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding new stories, validate phone numbers
</commit_message>
<xml_diff>
--- a/rasaproject8/user_data.xlsx
+++ b/rasaproject8/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,14 +561,97 @@
           <t>3323e32e342</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>382250162</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>my phone is not working</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>sewmina</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>536262547252464826325264746</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>my phone is not working</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>chulanjana</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>2424242424</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>our area has no signal and my internet connection is very slow,</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>chulanjana</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>0382250162</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>my phone is not working</t>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>our area has no signal and my internet connection is very slow, I want to record a complaint about it</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>chulanjana</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0782343434</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>your service is poor, about our area has no signal. and my internet connection is very slow</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>gihan bandara</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>200110312</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>you guys came to our place last week an fix my router issue. but again I'm facing the same issue can you please take action for it</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add a blame intent
</commit_message>
<xml_diff>
--- a/rasaproject8/user_data.xlsx
+++ b/rasaproject8/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -655,6 +655,11 @@
         </is>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
adding new stories and testing
</commit_message>
<xml_diff>
--- a/rasaproject8/user_data.xlsx
+++ b/rasaproject8/user_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -668,6 +668,36 @@
       </c>
       <c r="C15" t="inlineStr"/>
     </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>0777553527236346346523724y635u7</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0743555526</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>supun dissanayaka</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0382250162</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>my router is not working properly there is red light blinking on los bulb</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>